<commit_message>
Begin updating with year removed for BRT
</commit_message>
<xml_diff>
--- a/results/model_results.xlsx
+++ b/results/model_results.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Snow_CrabSDM\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECB34EE-8AD3-4654-A131-4A94ED89E40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829A07B2-A5AB-46AF-985C-8447AB40227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13530" yWindow="-13290" windowWidth="14340" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM" sheetId="1" r:id="rId1"/>
     <sheet name="BRT" sheetId="2" r:id="rId2"/>
-    <sheet name="RF" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="39">
   <si>
     <t>Formula</t>
   </si>
@@ -511,8 +510,8 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1406,8 +1405,8 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1470,19 +1469,19 @@
         <v>0.5</v>
       </c>
       <c r="F2">
-        <v>3.54</v>
+        <v>2.88</v>
       </c>
       <c r="G2">
-        <v>8.69</v>
+        <v>9.3179999999999996</v>
       </c>
       <c r="H2">
-        <v>0.9</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="I2">
-        <v>0.73</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="J2">
-        <v>550</v>
+        <v>850</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1501,20 +1500,20 @@
       <c r="E3">
         <v>0.5</v>
       </c>
-      <c r="F3">
-        <v>2.66</v>
-      </c>
-      <c r="G3">
-        <v>8.67</v>
-      </c>
-      <c r="H3">
-        <v>0.93</v>
-      </c>
-      <c r="I3">
-        <v>0.73</v>
-      </c>
-      <c r="J3">
-        <v>4150</v>
+      <c r="F3" s="9">
+        <v>3.1019999999999999</v>
+      </c>
+      <c r="G3" s="9">
+        <v>9.0250000000000004</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0.72</v>
+      </c>
+      <c r="J3" s="9">
+        <v>3700</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1534,19 +1533,19 @@
         <v>0.5</v>
       </c>
       <c r="F4">
-        <v>4.49</v>
+        <v>4.8230000000000004</v>
       </c>
       <c r="G4">
-        <v>8.8800000000000008</v>
+        <v>9.3789999999999996</v>
       </c>
       <c r="H4">
-        <v>0.87</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="I4">
-        <v>0.72</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="J4">
-        <v>3800</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1566,19 +1565,19 @@
         <v>0.5</v>
       </c>
       <c r="F5" s="8">
-        <v>3.12</v>
+        <v>2.3130000000000002</v>
       </c>
       <c r="G5" s="8">
-        <v>8.76</v>
+        <v>9.3510000000000009</v>
       </c>
       <c r="H5" s="8">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
       <c r="I5" s="8">
-        <v>0.73</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="J5" s="8">
-        <v>1350</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1598,19 +1597,19 @@
         <v>0.75</v>
       </c>
       <c r="F6">
-        <v>3.2</v>
+        <v>3.1989999999999998</v>
       </c>
       <c r="G6">
-        <v>8.74</v>
+        <v>9.01</v>
       </c>
       <c r="H6">
-        <v>0.92</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="I6">
-        <v>0.72</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="J6">
-        <v>2900</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1630,19 +1629,19 @@
         <v>0.25</v>
       </c>
       <c r="F7">
-        <v>3.95</v>
+        <v>2.3130000000000002</v>
       </c>
       <c r="G7">
-        <v>8.9</v>
+        <v>9.2669999999999995</v>
       </c>
       <c r="H7">
-        <v>0.89</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="I7">
-        <v>0.71</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="J7">
-        <v>2950</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1661,21 +1660,6 @@
       <c r="E8">
         <v>0.5</v>
       </c>
-      <c r="F8">
-        <v>2.54</v>
-      </c>
-      <c r="G8">
-        <v>4.34</v>
-      </c>
-      <c r="H8">
-        <v>0.85</v>
-      </c>
-      <c r="I8">
-        <v>0.72</v>
-      </c>
-      <c r="J8">
-        <v>250</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
@@ -1693,21 +1677,6 @@
       <c r="E9">
         <v>0.5</v>
       </c>
-      <c r="F9">
-        <v>2.42</v>
-      </c>
-      <c r="G9">
-        <v>4.41</v>
-      </c>
-      <c r="H9">
-        <v>0.86</v>
-      </c>
-      <c r="I9">
-        <v>0.71</v>
-      </c>
-      <c r="J9">
-        <v>1300</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
@@ -1725,21 +1694,6 @@
       <c r="E10">
         <v>0.5</v>
       </c>
-      <c r="F10">
-        <v>2.74</v>
-      </c>
-      <c r="G10">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="H10">
-        <v>0.84</v>
-      </c>
-      <c r="I10">
-        <v>0.71</v>
-      </c>
-      <c r="J10">
-        <v>1950</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
@@ -1748,29 +1702,14 @@
       <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11">
         <v>0.01</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11">
         <v>0.5</v>
-      </c>
-      <c r="F11" s="9">
-        <v>2.09</v>
-      </c>
-      <c r="G11" s="9">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0.88</v>
-      </c>
-      <c r="I11" s="9">
-        <v>0.72</v>
-      </c>
-      <c r="J11" s="9">
-        <v>750</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1789,21 +1728,11 @@
       <c r="E12" s="8">
         <v>0.75</v>
       </c>
-      <c r="F12" s="8">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G12" s="8">
-        <v>4.33</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0.87</v>
-      </c>
-      <c r="I12" s="8">
-        <v>0.72</v>
-      </c>
-      <c r="J12" s="8">
-        <v>1350</v>
-      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
@@ -1821,21 +1750,6 @@
       <c r="E13">
         <v>0.25</v>
       </c>
-      <c r="F13" s="9">
-        <v>2.41</v>
-      </c>
-      <c r="G13" s="9">
-        <v>4.3</v>
-      </c>
-      <c r="H13" s="9">
-        <v>0.86</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0.73</v>
-      </c>
-      <c r="J13" s="9">
-        <v>1700</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
@@ -1853,21 +1767,6 @@
       <c r="E14">
         <v>0.5</v>
       </c>
-      <c r="F14">
-        <v>2.77</v>
-      </c>
-      <c r="G14">
-        <v>4.41</v>
-      </c>
-      <c r="H14">
-        <v>0.73</v>
-      </c>
-      <c r="I14">
-        <v>0.45</v>
-      </c>
-      <c r="J14">
-        <v>200</v>
-      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
@@ -1885,21 +1784,6 @@
       <c r="E15">
         <v>0.5</v>
       </c>
-      <c r="F15">
-        <v>2.76</v>
-      </c>
-      <c r="G15">
-        <v>4.37</v>
-      </c>
-      <c r="H15">
-        <v>0.73</v>
-      </c>
-      <c r="I15">
-        <v>0.47</v>
-      </c>
-      <c r="J15">
-        <v>950</v>
-      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
@@ -1917,21 +1801,6 @@
       <c r="E16">
         <v>0.5</v>
       </c>
-      <c r="F16">
-        <v>3.1</v>
-      </c>
-      <c r="G16">
-        <v>4.45</v>
-      </c>
-      <c r="H16">
-        <v>0.68</v>
-      </c>
-      <c r="I16">
-        <v>0.45</v>
-      </c>
-      <c r="J16">
-        <v>1250</v>
-      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -1940,29 +1809,14 @@
       <c r="B17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17">
         <v>10</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17">
         <v>0.01</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17">
         <v>0.5</v>
-      </c>
-      <c r="F17" s="9">
-        <v>2.48</v>
-      </c>
-      <c r="G17" s="9">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0.77</v>
-      </c>
-      <c r="I17" s="9">
-        <v>0.46</v>
-      </c>
-      <c r="J17" s="9">
-        <v>550</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1981,21 +1835,11 @@
       <c r="E18" s="8">
         <v>0.75</v>
       </c>
-      <c r="F18" s="8">
-        <v>2.7</v>
-      </c>
-      <c r="G18" s="8">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="H18" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="I18" s="8">
-        <v>0.46</v>
-      </c>
-      <c r="J18" s="8">
-        <v>950</v>
-      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
@@ -2013,21 +1857,6 @@
       <c r="E19">
         <v>0.25</v>
       </c>
-      <c r="F19" s="9">
-        <v>2.66</v>
-      </c>
-      <c r="G19" s="9">
-        <v>4.38</v>
-      </c>
-      <c r="H19" s="9">
-        <v>0.74</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0.46</v>
-      </c>
-      <c r="J19" s="9">
-        <v>1400</v>
-      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
@@ -2045,21 +1874,6 @@
       <c r="E20">
         <v>0.5</v>
       </c>
-      <c r="F20" s="9">
-        <v>3.09</v>
-      </c>
-      <c r="G20" s="9">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="H20" s="9">
-        <v>0.82</v>
-      </c>
-      <c r="I20" s="9">
-        <v>0.68</v>
-      </c>
-      <c r="J20" s="9">
-        <v>200</v>
-      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
@@ -2077,21 +1891,6 @@
       <c r="E21">
         <v>0.5</v>
       </c>
-      <c r="F21" s="9">
-        <v>2.92</v>
-      </c>
-      <c r="G21" s="9">
-        <v>4.8</v>
-      </c>
-      <c r="H21" s="9">
-        <v>0.83</v>
-      </c>
-      <c r="I21" s="9">
-        <v>0.69</v>
-      </c>
-      <c r="J21" s="9">
-        <v>1150</v>
-      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
@@ -2109,21 +1908,6 @@
       <c r="E22">
         <v>0.5</v>
       </c>
-      <c r="F22" s="9">
-        <v>3.01</v>
-      </c>
-      <c r="G22" s="9">
-        <v>4.79</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0.82</v>
-      </c>
-      <c r="I22" s="9">
-        <v>0.69</v>
-      </c>
-      <c r="J22" s="9">
-        <v>2100</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
@@ -2132,29 +1916,14 @@
       <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23">
         <v>10</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>0.01</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23">
         <v>0.5</v>
-      </c>
-      <c r="F23" s="9">
-        <v>2.36</v>
-      </c>
-      <c r="G23" s="9">
-        <v>4.76</v>
-      </c>
-      <c r="H23" s="9">
-        <v>0.87</v>
-      </c>
-      <c r="I23" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="J23" s="9">
-        <v>800</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -2173,21 +1942,11 @@
       <c r="E24" s="8">
         <v>0.75</v>
       </c>
-      <c r="F24" s="8">
-        <v>2.54</v>
-      </c>
-      <c r="G24" s="8">
-        <v>4.78</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0.86</v>
-      </c>
-      <c r="I24" s="8">
-        <v>0.69</v>
-      </c>
-      <c r="J24" s="8">
-        <v>1500</v>
-      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
@@ -2204,240 +1963,10 @@
       </c>
       <c r="E25">
         <v>0.25</v>
-      </c>
-      <c r="F25" s="9">
-        <v>2.97</v>
-      </c>
-      <c r="G25" s="9">
-        <v>4.7</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0.83</v>
-      </c>
-      <c r="I25" s="9">
-        <v>0.69</v>
-      </c>
-      <c r="J25" s="9">
-        <v>1350</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8C35A5-F040-491B-9D9F-4E0B7840D57B}">
-  <dimension ref="A1:B25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
New model results tab
</commit_message>
<xml_diff>
--- a/results/model_results.xlsx
+++ b/results/model_results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Snow_CrabSDM\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11868508-873E-4C6B-85FA-2670F1014851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529ED1B1-B78C-4999-9111-EC67472DF27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="-16185" windowWidth="19125" windowHeight="10035" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GAM" sheetId="1" r:id="rId1"/>
     <sheet name="BRT" sheetId="2" r:id="rId2"/>
+    <sheet name="Model Comparison" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="57">
   <si>
     <t>Formula</t>
   </si>
@@ -130,19 +131,73 @@
     <t>Bag Fraction</t>
   </si>
   <si>
-    <t>Residual Deviance</t>
-  </si>
-  <si>
-    <t>Trees</t>
-  </si>
-  <si>
-    <t>CV Deviance</t>
-  </si>
-  <si>
-    <t>Training Correlation</t>
-  </si>
-  <si>
-    <t>CV Correlation</t>
+    <t>Mature Female</t>
+  </si>
+  <si>
+    <t>Immature Female</t>
+  </si>
+  <si>
+    <t>Legal Male</t>
+  </si>
+  <si>
+    <t>Sublegal Male</t>
+  </si>
+  <si>
+    <t>GAM (Tweedie)</t>
+  </si>
+  <si>
+    <t>GAM (delta)</t>
+  </si>
+  <si>
+    <t>BRT</t>
+  </si>
+  <si>
+    <t>RMSE Table</t>
+  </si>
+  <si>
+    <t>Deviance Explained</t>
+  </si>
+  <si>
+    <t>Max Trees</t>
+  </si>
+  <si>
+    <t>Step Size</t>
+  </si>
+  <si>
+    <t>Number Trees</t>
+  </si>
+  <si>
+    <t>Mature Female (Bernoulli)</t>
+  </si>
+  <si>
+    <t>Mature Female (Gaussian)</t>
+  </si>
+  <si>
+    <t>33.4% (51.2%)</t>
+  </si>
+  <si>
+    <t>48.1% (44.1%)</t>
+  </si>
+  <si>
+    <t>41.8% (56.0%)</t>
+  </si>
+  <si>
+    <t>61.0% (59.9%)</t>
+  </si>
+  <si>
+    <t>53.4% (58.6%)</t>
+  </si>
+  <si>
+    <t>Immature Female (Bernoulli)</t>
+  </si>
+  <si>
+    <t>Immature Female (Gaussian)</t>
+  </si>
+  <si>
+    <t>* number in parentheses is presence model</t>
+  </si>
+  <si>
+    <t>63.2% (54.3%)</t>
   </si>
 </sst>
 </file>
@@ -166,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,18 +252,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -222,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -231,15 +274,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF49956F"/>
+      <color rgb="FFFBA96B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -249,6 +296,1073 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>RMSE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Model Comparison'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GAM (Tweedie)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Model Comparison'!$B$4:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mature Female</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Immature Female</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Legal Male</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sublegal Male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Model Comparison'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E88A-4E50-933E-105205D05FC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Model Comparison'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GAM (delta)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FBA96B"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Model Comparison'!$B$4:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mature Female</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Immature Female</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Legal Male</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sublegal Male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Model Comparison'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.119999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E88A-4E50-933E-105205D05FC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Model Comparison'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BRT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="49956F"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Model Comparison'!$B$4:$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Mature Female</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Immature Female</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Legal Male</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sublegal Male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Model Comparison'!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E88A-4E50-933E-105205D05FC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1212565696"/>
+        <c:axId val="1212566176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1212565696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1212566176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1212566176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1212565696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>422275</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>517525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E59400-4AC1-2209-DDCB-782B4A98A973}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1411,13 +2525,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28747FF-1FB7-4EF0-9863-442B02C2FB9C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="25.08984375" customWidth="1"/>
     <col min="3" max="3" width="13.90625" customWidth="1"/>
     <col min="4" max="4" width="12.6328125" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
@@ -1444,489 +2559,313 @@
         <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>23</v>
+      <c r="B2" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F2">
-        <v>0.60399999999999998</v>
+        <v>2000</v>
       </c>
       <c r="G2">
-        <v>1.5880000000000001</v>
+        <v>50</v>
       </c>
       <c r="H2">
-        <v>0.94199999999999995</v>
+        <v>2000</v>
       </c>
       <c r="I2">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="J2">
-        <v>2850</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>0.01</v>
-      </c>
-      <c r="E3">
-        <v>0.5</v>
-      </c>
-      <c r="F3">
-        <v>0.86</v>
-      </c>
-      <c r="G3">
-        <v>1.587</v>
-      </c>
-      <c r="H3">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="I3">
-        <v>0.83399999999999996</v>
-      </c>
-      <c r="J3">
-        <v>7700</v>
-      </c>
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2000</v>
+      </c>
+      <c r="G3" s="8">
+        <v>50</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1400</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.37</v>
+      </c>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>0.05</v>
-      </c>
-      <c r="E4">
-        <v>0.5</v>
-      </c>
-      <c r="F4">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="G4">
-        <v>1.5580000000000001</v>
-      </c>
-      <c r="H4">
-        <v>0.95399999999999996</v>
-      </c>
-      <c r="I4">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="J4">
-        <v>2400</v>
-      </c>
+      <c r="B4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="8">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="8">
+        <v>50</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2000</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="B5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="8">
         <v>10</v>
       </c>
-      <c r="D5" s="10">
-        <v>0.05</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="8">
         <v>0.5</v>
       </c>
-      <c r="F5" s="10">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="G5" s="10">
-        <v>1.5269999999999999</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.95699999999999996</v>
-      </c>
-      <c r="I5" s="10">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="J5" s="10">
-        <v>1600</v>
-      </c>
+      <c r="F5" s="8">
+        <v>2000</v>
+      </c>
+      <c r="G5" s="8">
+        <v>50</v>
+      </c>
+      <c r="H5" s="8">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.81</v>
+      </c>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>0.05</v>
-      </c>
-      <c r="E6">
-        <v>0.75</v>
-      </c>
-      <c r="F6">
-        <v>0.54300000000000004</v>
-      </c>
-      <c r="G6">
-        <v>1.544</v>
-      </c>
-      <c r="H6">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="I6">
-        <v>0.84</v>
-      </c>
-      <c r="J6">
-        <v>2950</v>
-      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>0.05</v>
-      </c>
-      <c r="E7">
-        <v>0.25</v>
-      </c>
-      <c r="F7">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="G7">
-        <v>1.6339999999999999</v>
-      </c>
-      <c r="H7">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="I7">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="J7">
-        <v>2950</v>
-      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>0.05</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <v>0.433</v>
-      </c>
-      <c r="G8">
-        <v>1.1559999999999999</v>
-      </c>
-      <c r="H8">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="I8">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="J8">
-        <v>3150</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>0.01</v>
-      </c>
-      <c r="E9">
-        <v>0.5</v>
-      </c>
-      <c r="F9">
-        <v>0.67</v>
-      </c>
-      <c r="G9">
-        <v>1.169</v>
-      </c>
-      <c r="H9">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="I9">
-        <v>0.85</v>
-      </c>
-      <c r="J9">
-        <v>6950</v>
-      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>0.01</v>
-      </c>
-      <c r="E10">
-        <v>0.5</v>
-      </c>
-      <c r="F10">
-        <v>0.375</v>
-      </c>
-      <c r="G10">
-        <v>1.121</v>
-      </c>
-      <c r="H10">
-        <v>0.95599999999999996</v>
-      </c>
-      <c r="I10">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="J10">
-        <v>2200</v>
-      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="10">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="E11" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="10">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="G11" s="10">
-        <v>1.0780000000000001</v>
-      </c>
-      <c r="H11" s="10">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="I11" s="10">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="J11" s="10">
-        <v>1950</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="9">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0.75</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1.1559999999999999</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0.85299999999999998</v>
-      </c>
-      <c r="J12" s="9">
-        <v>2950</v>
-      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>0.01</v>
-      </c>
-      <c r="E13">
-        <v>0.25</v>
-      </c>
-      <c r="F13">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="G13">
-        <v>1.169</v>
-      </c>
-      <c r="H13">
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="I13">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="J13">
-        <v>3850</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>0.05</v>
-      </c>
-      <c r="E14">
-        <v>0.5</v>
-      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>0.01</v>
-      </c>
-      <c r="E15">
-        <v>0.5</v>
-      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>0.01</v>
-      </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>0.01</v>
-      </c>
-      <c r="E17">
-        <v>0.5</v>
-      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="8">
-        <v>5</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0.75</v>
-      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1937,103 +2876,80 @@
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>0.01</v>
-      </c>
-      <c r="E19">
-        <v>0.25</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <v>0.05</v>
-      </c>
-      <c r="E20">
-        <v>0.5</v>
-      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>0.01</v>
-      </c>
-      <c r="E21">
-        <v>0.5</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>0.01</v>
-      </c>
-      <c r="E22">
-        <v>0.5</v>
-      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <v>0.01</v>
-      </c>
-      <c r="E23">
-        <v>0.5</v>
-      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="8">
-        <v>5</v>
-      </c>
-      <c r="D24" s="8">
-        <v>0.01</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0.75</v>
-      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -2044,21 +2960,170 @@
       <c r="A25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25">
-        <v>5</v>
-      </c>
-      <c r="D25">
-        <v>0.01</v>
-      </c>
-      <c r="E25">
-        <v>0.25</v>
-      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E502E113-8B3D-455D-A134-6030657C990C}">
+  <dimension ref="B1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>2.8</v>
+      </c>
+      <c r="D4">
+        <v>3.59</v>
+      </c>
+      <c r="E4">
+        <v>1.54</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="D5">
+        <v>2.59</v>
+      </c>
+      <c r="E5">
+        <v>1.41</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1.74</v>
+      </c>
+      <c r="D6">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>2.23</v>
+      </c>
+      <c r="D7">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Save and use RMSE plot
</commit_message>
<xml_diff>
--- a/results/model_results.xlsx
+++ b/results/model_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Snow_CrabSDM\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAF2651-C4EC-4574-BBCC-57DFD0B91C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B580F9-354E-4B3A-BBE0-A81F7A5548A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2914,7 +2914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E502E113-8B3D-455D-A134-6030657C990C}">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add RMSE from forecasts
</commit_message>
<xml_diff>
--- a/results/model_results.xlsx
+++ b/results/model_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Snow_CrabSDM\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B580F9-354E-4B3A-BBE0-A81F7A5548A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18793320-BDF4-4A1E-B7BE-AD7F587DABB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="GAM" sheetId="1" r:id="rId1"/>
     <sheet name="BRT" sheetId="2" r:id="rId2"/>
     <sheet name="Model Comparison" sheetId="3" r:id="rId3"/>
+    <sheet name="Forecast" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="71">
   <si>
     <t>Formula</t>
   </si>
@@ -234,6 +235,12 @@
   </si>
   <si>
     <t>48.9% (59.7%)</t>
+  </si>
+  <si>
+    <t>BRT (full)</t>
+  </si>
+  <si>
+    <t>BRT (forecast)</t>
   </si>
 </sst>
 </file>
@@ -2914,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E502E113-8B3D-455D-A134-6030657C990C}">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3159,4 +3166,81 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8220CFE4-3936-4A88-B5F4-62055CA5BCB2}">
+  <dimension ref="B1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>1.68</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>1.41</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1.25</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>1.6</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>